<commit_message>
Track block light signal re-implemented as a bool, crossing signal also implemented as a bool (none, false, true) to fit with track controller plc code.
</commit_message>
<xml_diff>
--- a/system_data/lines/red_line.xlsx
+++ b/system_data/lines/red_line.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d0c4a204f81830ef/Pitt/2024_Summer_Term/ECE 1140/Project/train_system/system_data/lines/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_F25DC773A252ABDACC104823A11D487E5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94D73715-FB55-457D-98ED-4CA3B8AFA400}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="11_F25DC773A252ABDACC104823A11D487E5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6649D798-2E02-48F8-ABDC-6CF72450A922}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="14630" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="25600" windowHeight="15250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="65">
   <si>
     <t>Line</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Underground</t>
   </si>
   <si>
-    <t>Crossing</t>
-  </si>
-  <si>
     <t>Station</t>
   </si>
   <si>
@@ -217,6 +214,12 @@
   </si>
   <si>
     <t>9, 10, 78</t>
+  </si>
+  <si>
+    <t>Crossing Signal</t>
+  </si>
+  <si>
+    <t>Light Signal</t>
   </si>
 </sst>
 </file>
@@ -571,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L154"/>
+  <dimension ref="A1:M154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C49" workbookViewId="0">
-      <selection activeCell="L80" sqref="L80"/>
+    <sheetView tabSelected="1" topLeftCell="B47" workbookViewId="0">
+      <selection activeCell="K79" sqref="K79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -587,12 +590,12 @@
     <col min="7" max="7" width="8.81640625" style="7"/>
     <col min="8" max="8" width="14.453125" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
-    <col min="10" max="10" width="10.36328125" customWidth="1"/>
-    <col min="11" max="11" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.7265625" customWidth="1"/>
+    <col min="10" max="11" width="10.36328125" customWidth="1"/>
+    <col min="12" max="12" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -621,21 +624,24 @@
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="C2" s="4">
         <v>1</v>
@@ -661,18 +667,21 @@
       <c r="J2" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="str">
         <f>A2</f>
         <v>Red</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="3">
         <v>2</v>
@@ -698,19 +707,22 @@
       <c r="J3" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3" t="str">
+      <c r="K3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3" t="str">
         <f>C2&amp;", "&amp;C4</f>
         <v>1, 3</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="str">
         <f t="shared" ref="A4:A67" si="0">A3</f>
         <v>Red</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="3">
         <v>3</v>
@@ -736,19 +748,22 @@
       <c r="J4" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3" t="str">
-        <f t="shared" ref="L4:L15" si="1">C3&amp;", "&amp;C5</f>
+      <c r="K4" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3" t="str">
+        <f t="shared" ref="M4:M15" si="1">C3&amp;", "&amp;C5</f>
         <v>2, 4</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="4">
         <v>4</v>
@@ -774,19 +789,22 @@
       <c r="J5" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3" t="str">
+      <c r="K5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3" t="str">
         <f t="shared" si="1"/>
         <v>3, 5</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="3">
         <v>5</v>
@@ -812,19 +830,22 @@
       <c r="J6" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3" t="str">
+      <c r="K6" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3" t="str">
         <f t="shared" si="1"/>
         <v>4, 6</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="3">
         <v>6</v>
@@ -850,19 +871,22 @@
       <c r="J7" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3" t="str">
+      <c r="K7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3" t="str">
         <f t="shared" si="1"/>
         <v>5, 7</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="4">
         <v>7</v>
@@ -888,21 +912,24 @@
       <c r="J8" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="L8" s="3" t="str">
+      <c r="K8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M8" s="3" t="str">
         <f t="shared" si="1"/>
         <v>6, 8</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="3">
         <v>8</v>
@@ -928,19 +955,22 @@
       <c r="J9" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3" t="str">
+      <c r="K9" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3" t="str">
         <f t="shared" si="1"/>
         <v>7, 9</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="3">
         <v>9</v>
@@ -966,18 +996,21 @@
       <c r="J10" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K10" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="4">
         <v>10</v>
@@ -1003,18 +1036,21 @@
       <c r="J11" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K11" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="3">
         <v>11</v>
@@ -1040,19 +1076,22 @@
       <c r="J12" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3" t="str">
+      <c r="K12" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3" t="str">
         <f t="shared" si="1"/>
         <v>10, 12</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="4">
         <v>12</v>
@@ -1078,19 +1117,22 @@
       <c r="J13" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3" t="str">
+      <c r="K13" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3" t="str">
         <f t="shared" si="1"/>
         <v>11, 13</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="3">
         <v>13</v>
@@ -1116,19 +1158,22 @@
       <c r="J14" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3" t="str">
+      <c r="K14" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3" t="str">
         <f t="shared" si="1"/>
         <v>12, 14</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="3">
         <v>14</v>
@@ -1154,19 +1199,22 @@
       <c r="J15" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3" t="str">
+      <c r="K15" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3" t="str">
         <f t="shared" si="1"/>
         <v>13, 15</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="4">
         <v>15</v>
@@ -1192,18 +1240,21 @@
       <c r="J16" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K16" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" s="3">
         <v>16</v>
@@ -1229,20 +1280,23 @@
       <c r="J17" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K17" s="3" t="s">
-        <v>34</v>
+      <c r="K17" s="3" t="b">
+        <v>1</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" s="4">
         <v>17</v>
@@ -1268,19 +1322,22 @@
       <c r="J18" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3" t="str">
-        <f t="shared" ref="L18:L38" si="2">C17&amp;", "&amp;C19</f>
+      <c r="K18" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3" t="str">
+        <f t="shared" ref="M18:M38" si="2">C17&amp;", "&amp;C19</f>
         <v>16, 18</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" s="3">
         <v>18</v>
@@ -1307,19 +1364,22 @@
       <c r="J19" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3" t="str">
+      <c r="K19" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3" t="str">
         <f t="shared" si="2"/>
         <v>17, 19</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" s="3">
         <v>19</v>
@@ -1345,19 +1405,22 @@
       <c r="J20" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3" t="str">
+      <c r="K20" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3" t="str">
         <f t="shared" si="2"/>
         <v>18, 20</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C21" s="4">
         <v>20</v>
@@ -1383,19 +1446,22 @@
       <c r="J21" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3" t="str">
+      <c r="K21" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3" t="str">
         <f t="shared" si="2"/>
         <v>19, 21</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C22" s="3">
         <v>21</v>
@@ -1421,21 +1487,24 @@
       <c r="J22" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K22" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="L22" s="3" t="str">
+      <c r="K22" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M22" s="3" t="str">
         <f t="shared" si="2"/>
         <v>20, 22</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C23" s="4">
         <v>22</v>
@@ -1461,19 +1530,22 @@
       <c r="J23" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3" t="str">
+      <c r="K23" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3" t="str">
         <f t="shared" si="2"/>
         <v>21, 23</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C24" s="3">
         <v>23</v>
@@ -1499,19 +1571,22 @@
       <c r="J24" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3" t="str">
+      <c r="K24" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3" t="str">
         <f t="shared" si="2"/>
         <v>22, 24</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C25" s="3">
         <v>24</v>
@@ -1537,19 +1612,22 @@
       <c r="J25" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3" t="str">
+      <c r="K25" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3" t="str">
         <f t="shared" si="2"/>
         <v>23, 25</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C26" s="4">
         <v>25</v>
@@ -1575,21 +1653,24 @@
       <c r="J26" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K26" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="L26" s="3" t="str">
+      <c r="K26" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M26" s="3" t="str">
         <f t="shared" si="2"/>
         <v>24, 26</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C27" s="3">
         <v>26</v>
@@ -1615,19 +1696,22 @@
       <c r="J27" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3" t="str">
+      <c r="K27" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3" t="str">
         <f t="shared" si="2"/>
         <v>25, 27</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C28" s="4">
         <v>27</v>
@@ -1653,18 +1737,21 @@
       <c r="J28" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K28" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C29" s="3">
         <v>28</v>
@@ -1690,18 +1777,21 @@
       <c r="J29" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K29" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C30" s="3">
         <v>29</v>
@@ -1727,19 +1817,22 @@
       <c r="J30" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3" t="str">
+      <c r="K30" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3" t="str">
         <f t="shared" si="2"/>
         <v>28, 30</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C31" s="4">
         <v>30</v>
@@ -1765,19 +1858,22 @@
       <c r="J31" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3" t="str">
+      <c r="K31" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3" t="str">
         <f t="shared" si="2"/>
         <v>29, 31</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C32" s="3">
         <v>31</v>
@@ -1803,19 +1899,22 @@
       <c r="J32" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3" t="str">
+      <c r="K32" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3" t="str">
         <f t="shared" si="2"/>
         <v>30, 32</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C33" s="4">
         <v>32</v>
@@ -1841,18 +1940,21 @@
       <c r="J33" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K33" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C34" s="3">
         <v>33</v>
@@ -1878,18 +1980,21 @@
       <c r="J34" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K34" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C35" s="3">
         <v>34</v>
@@ -1915,19 +2020,22 @@
       <c r="J35" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3" t="str">
+      <c r="K35" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3" t="str">
         <f t="shared" si="2"/>
         <v>33, 35</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C36" s="4">
         <v>35</v>
@@ -1953,21 +2061,24 @@
       <c r="J36" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K36" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="L36" s="3" t="str">
+      <c r="K36" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L36" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="M36" s="3" t="str">
         <f t="shared" si="2"/>
         <v>34, 36</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C37" s="3">
         <v>36</v>
@@ -1993,19 +2104,22 @@
       <c r="J37" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3" t="str">
+      <c r="K37" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3" t="str">
         <f t="shared" si="2"/>
         <v>35, 37</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C38" s="3">
         <v>37</v>
@@ -2031,19 +2145,22 @@
       <c r="J38" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3" t="str">
+      <c r="K38" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3" t="str">
         <f t="shared" si="2"/>
         <v>36, 38</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C39" s="4">
         <v>38</v>
@@ -2069,18 +2186,21 @@
       <c r="J39" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K39" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C40" s="3">
         <v>39</v>
@@ -2106,18 +2226,21 @@
       <c r="J40" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K40" s="3"/>
-      <c r="L40" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K40" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C41" s="3">
         <v>40</v>
@@ -2143,19 +2266,22 @@
       <c r="J41" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K41" s="3"/>
-      <c r="L41" s="3" t="str">
-        <f t="shared" ref="L41:L43" si="3">C40&amp;", "&amp;C42</f>
+      <c r="K41" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3" t="str">
+        <f t="shared" ref="M41:M43" si="3">C40&amp;", "&amp;C42</f>
         <v>39, 41</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C42" s="4">
         <v>41</v>
@@ -2181,19 +2307,22 @@
       <c r="J42" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K42" s="3"/>
-      <c r="L42" s="3" t="str">
+      <c r="K42" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3" t="str">
         <f t="shared" si="3"/>
         <v>40, 42</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C43" s="3">
         <v>42</v>
@@ -2219,19 +2348,22 @@
       <c r="J43" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K43" s="3"/>
-      <c r="L43" s="3" t="str">
+      <c r="K43" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3" t="str">
         <f t="shared" si="3"/>
         <v>41, 43</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C44" s="3">
         <v>43</v>
@@ -2257,18 +2389,21 @@
       <c r="J44" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K44" s="3"/>
-      <c r="L44" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K44" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L44" s="3"/>
+      <c r="M44" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C45" s="4">
         <v>44</v>
@@ -2294,18 +2429,21 @@
       <c r="J45" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K45" s="3"/>
-      <c r="L45" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K45" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L45" s="3"/>
+      <c r="M45" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C46" s="3">
         <v>45</v>
@@ -2331,21 +2469,24 @@
       <c r="J46" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K46" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="L46" s="3" t="str">
-        <f t="shared" ref="L46:L52" si="4">C45&amp;", "&amp;C47</f>
+      <c r="K46" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L46" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M46" s="3" t="str">
+        <f t="shared" ref="M46:M52" si="4">C45&amp;", "&amp;C47</f>
         <v>44, 46</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C47" s="3">
         <v>46</v>
@@ -2371,19 +2512,22 @@
       <c r="J47" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K47" s="3"/>
-      <c r="L47" s="3" t="str">
+      <c r="K47" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L47" s="3"/>
+      <c r="M47" s="3" t="str">
         <f t="shared" si="4"/>
         <v>45, 47</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C48" s="4">
         <v>47</v>
@@ -2409,19 +2553,22 @@
       <c r="J48" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="K48" s="3"/>
-      <c r="L48" s="3" t="str">
+      <c r="K48" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L48" s="3"/>
+      <c r="M48" s="3" t="str">
         <f t="shared" si="4"/>
         <v>46, 48</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C49" s="3">
         <v>48</v>
@@ -2447,21 +2594,24 @@
       <c r="J49" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K49" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="L49" s="3" t="str">
+      <c r="K49" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L49" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M49" s="3" t="str">
         <f t="shared" si="4"/>
         <v>47, 49</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C50" s="3">
         <v>49</v>
@@ -2487,19 +2637,22 @@
       <c r="J50" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K50" s="3"/>
-      <c r="L50" s="3" t="str">
+      <c r="K50" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L50" s="3"/>
+      <c r="M50" s="3" t="str">
         <f t="shared" si="4"/>
         <v>48, 50</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C51" s="4">
         <v>50</v>
@@ -2525,19 +2678,22 @@
       <c r="J51" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K51" s="3"/>
-      <c r="L51" s="3" t="str">
+      <c r="K51" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L51" s="3"/>
+      <c r="M51" s="3" t="str">
         <f t="shared" si="4"/>
         <v>49, 51</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C52" s="3">
         <v>51</v>
@@ -2563,19 +2719,22 @@
       <c r="J52" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K52" s="3"/>
-      <c r="L52" s="3" t="str">
+      <c r="K52" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L52" s="3"/>
+      <c r="M52" s="3" t="str">
         <f t="shared" si="4"/>
         <v>50, 52</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C53" s="3">
         <v>52</v>
@@ -2601,18 +2760,21 @@
       <c r="J53" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K53" s="3"/>
-      <c r="L53" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K53" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L53" s="3"/>
+      <c r="M53" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C54" s="4">
         <v>53</v>
@@ -2638,18 +2800,21 @@
       <c r="J54" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K54" s="3"/>
-      <c r="L54" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K54" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L54" s="3"/>
+      <c r="M54" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C55" s="3">
         <v>54</v>
@@ -2675,19 +2840,22 @@
       <c r="J55" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K55" s="3"/>
-      <c r="L55" s="3" t="str">
-        <f t="shared" ref="L55:L66" si="5">C54&amp;", "&amp;C56</f>
+      <c r="K55" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L55" s="3"/>
+      <c r="M55" s="3" t="str">
+        <f t="shared" ref="M55:M66" si="5">C54&amp;", "&amp;C56</f>
         <v>53, 55</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C56" s="3">
         <v>55</v>
@@ -2713,19 +2881,22 @@
       <c r="J56" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K56" s="3"/>
-      <c r="L56" s="3" t="str">
+      <c r="K56" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L56" s="3"/>
+      <c r="M56" s="3" t="str">
         <f t="shared" si="5"/>
         <v>54, 56</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C57" s="4">
         <v>56</v>
@@ -2751,19 +2922,22 @@
       <c r="J57" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K57" s="3"/>
-      <c r="L57" s="3" t="str">
+      <c r="K57" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L57" s="3"/>
+      <c r="M57" s="3" t="str">
         <f t="shared" si="5"/>
         <v>55, 57</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C58" s="3">
         <v>57</v>
@@ -2789,19 +2963,22 @@
       <c r="J58" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K58" s="3"/>
-      <c r="L58" s="3" t="str">
+      <c r="K58" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L58" s="3"/>
+      <c r="M58" s="3" t="str">
         <f t="shared" si="5"/>
         <v>56, 58</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C59" s="3">
         <v>58</v>
@@ -2827,19 +3004,22 @@
       <c r="J59" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K59" s="3"/>
-      <c r="L59" s="3" t="str">
+      <c r="K59" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L59" s="3"/>
+      <c r="M59" s="3" t="str">
         <f t="shared" si="5"/>
         <v>57, 59</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C60" s="4">
         <v>59</v>
@@ -2865,19 +3045,22 @@
       <c r="J60" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K60" s="3"/>
-      <c r="L60" s="3" t="str">
+      <c r="K60" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L60" s="3"/>
+      <c r="M60" s="3" t="str">
         <f t="shared" si="5"/>
         <v>58, 60</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C61" s="3">
         <v>60</v>
@@ -2903,21 +3086,24 @@
       <c r="J61" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K61" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="L61" s="3" t="str">
+      <c r="K61" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L61" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M61" s="3" t="str">
         <f t="shared" si="5"/>
         <v>59, 61</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C62" s="3">
         <v>61</v>
@@ -2943,19 +3129,22 @@
       <c r="J62" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K62" s="3"/>
-      <c r="L62" s="3" t="str">
+      <c r="K62" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L62" s="3"/>
+      <c r="M62" s="3" t="str">
         <f t="shared" si="5"/>
         <v>60, 62</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C63" s="4">
         <v>62</v>
@@ -2981,19 +3170,22 @@
       <c r="J63" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K63" s="3"/>
-      <c r="L63" s="3" t="str">
+      <c r="K63" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L63" s="3"/>
+      <c r="M63" s="3" t="str">
         <f t="shared" si="5"/>
         <v>61, 63</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C64" s="3">
         <v>63</v>
@@ -3019,19 +3211,22 @@
       <c r="J64" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K64" s="3"/>
-      <c r="L64" s="3" t="str">
+      <c r="K64" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L64" s="3"/>
+      <c r="M64" s="3" t="str">
         <f t="shared" si="5"/>
         <v>62, 64</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C65" s="3">
         <v>64</v>
@@ -3057,19 +3252,22 @@
       <c r="J65" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K65" s="3"/>
-      <c r="L65" s="3" t="str">
+      <c r="K65" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L65" s="3"/>
+      <c r="M65" s="3" t="str">
         <f t="shared" si="5"/>
         <v>63, 65</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C66" s="4">
         <v>65</v>
@@ -3095,19 +3293,22 @@
       <c r="J66" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K66" s="3"/>
-      <c r="L66" s="3" t="str">
+      <c r="K66" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L66" s="3"/>
+      <c r="M66" s="3" t="str">
         <f t="shared" si="5"/>
         <v>64, 66</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C67" s="3">
         <v>66</v>
@@ -3133,18 +3334,21 @@
       <c r="J67" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K67" s="3"/>
-      <c r="L67" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K67" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L67" s="3"/>
+      <c r="M67" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="str">
         <f t="shared" ref="A68:A79" si="6">A67</f>
         <v>Red</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C68" s="3">
         <v>67</v>
@@ -3170,18 +3374,21 @@
       <c r="J68" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K68" s="3"/>
-      <c r="L68" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K68" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L68" s="3"/>
+      <c r="M68" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="str">
         <f t="shared" si="6"/>
         <v>Red</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C69" s="4">
         <v>68</v>
@@ -3207,19 +3414,22 @@
       <c r="J69" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K69" s="3"/>
-      <c r="L69" s="3" t="str">
-        <f t="shared" ref="L69:L71" si="7">C68&amp;", "&amp;C70</f>
+      <c r="K69" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L69" s="3"/>
+      <c r="M69" s="3" t="str">
+        <f t="shared" ref="M69:M71" si="7">C68&amp;", "&amp;C70</f>
         <v>67, 69</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="str">
         <f t="shared" si="6"/>
         <v>Red</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C70" s="3">
         <v>69</v>
@@ -3245,19 +3455,22 @@
       <c r="J70" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K70" s="3"/>
-      <c r="L70" s="3" t="str">
+      <c r="K70" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L70" s="3"/>
+      <c r="M70" s="3" t="str">
         <f t="shared" si="7"/>
         <v>68, 70</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="str">
         <f t="shared" si="6"/>
         <v>Red</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C71" s="3">
         <v>70</v>
@@ -3283,19 +3496,22 @@
       <c r="J71" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K71" s="3"/>
-      <c r="L71" s="3" t="str">
+      <c r="K71" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L71" s="3"/>
+      <c r="M71" s="3" t="str">
         <f t="shared" si="7"/>
         <v>69, 71</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="str">
         <f t="shared" si="6"/>
         <v>Red</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C72" s="4">
         <v>71</v>
@@ -3321,18 +3537,21 @@
       <c r="J72" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K72" s="3"/>
-      <c r="L72" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K72" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L72" s="3"/>
+      <c r="M72" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="str">
         <f t="shared" si="6"/>
         <v>Red</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C73" s="3">
         <v>72</v>
@@ -3358,18 +3577,21 @@
       <c r="J73" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K73" s="3"/>
-      <c r="L73" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K73" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L73" s="3"/>
+      <c r="M73" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A74" s="3" t="str">
         <f t="shared" si="6"/>
         <v>Red</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C74" s="3">
         <v>73</v>
@@ -3395,19 +3617,22 @@
       <c r="J74" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K74" s="3"/>
-      <c r="L74" s="3" t="str">
-        <f t="shared" ref="L74:L76" si="8">C73&amp;", "&amp;C75</f>
+      <c r="K74" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L74" s="3"/>
+      <c r="M74" s="3" t="str">
+        <f t="shared" ref="M74:M76" si="8">C73&amp;", "&amp;C75</f>
         <v>72, 74</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="str">
         <f t="shared" si="6"/>
         <v>Red</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C75" s="4">
         <v>74</v>
@@ -3433,19 +3658,22 @@
       <c r="J75" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K75" s="3"/>
-      <c r="L75" s="3" t="str">
+      <c r="K75" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L75" s="3"/>
+      <c r="M75" s="3" t="str">
         <f t="shared" si="8"/>
         <v>73, 75</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="str">
         <f t="shared" si="6"/>
         <v>Red</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C76" s="3">
         <v>75</v>
@@ -3471,19 +3699,22 @@
       <c r="J76" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K76" s="3"/>
-      <c r="L76" s="3" t="str">
+      <c r="K76" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L76" s="3"/>
+      <c r="M76" s="3" t="str">
         <f t="shared" si="8"/>
         <v>74, 76</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A77" s="3" t="str">
         <f t="shared" si="6"/>
         <v>Red</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C77" s="3">
         <v>76</v>
@@ -3509,18 +3740,21 @@
       <c r="J77" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K77" s="3"/>
-      <c r="L77" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K77" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L77" s="3"/>
+      <c r="M77" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="str">
         <f t="shared" si="6"/>
         <v>Red</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C78" s="4">
         <v>77</v>
@@ -3546,18 +3780,21 @@
       <c r="J78" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K78" s="3"/>
-      <c r="L78" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K78" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L78" s="3"/>
+      <c r="M78" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="str">
         <f t="shared" si="6"/>
         <v>Red</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C79" s="4">
         <v>78</v>
@@ -3584,11 +3821,12 @@
         <v>0</v>
       </c>
       <c r="K79" s="3"/>
-      <c r="L79" s="3">
+      <c r="L79" s="3"/>
+      <c r="M79" s="3">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C80" s="6"/>
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated signals in red line excel
</commit_message>
<xml_diff>
--- a/system_data/lines/red_line.xlsx
+++ b/system_data/lines/red_line.xlsx
@@ -5,27 +5,38 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d0c4a204f81830ef/Pitt/2024_Summer_Term/ECE 1140/Project/train_system/system_data/lines/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isabella\Trains\train_system\system_data\lines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="11_F25DC773A252ABDACC104823A11D487E5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6649D798-2E02-48F8-ABDC-6CF72450A922}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E560744-A9E1-4D82-9ACF-D1821D77D26F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="25600" windowHeight="15250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="67">
   <si>
     <t>Line</t>
   </si>
@@ -220,6 +231,12 @@
   </si>
   <si>
     <t>Light Signal</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>False</t>
   </si>
 </sst>
 </file>
@@ -270,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -292,6 +309,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -576,26 +596,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B47" workbookViewId="0">
-      <selection activeCell="K79" sqref="K79"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.81640625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" style="5" customWidth="1"/>
     <col min="4" max="4" width="11" style="5" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="13.26953125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="8.81640625" style="7"/>
-    <col min="8" max="8" width="14.453125" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="8.77734375" style="7"/>
+    <col min="8" max="8" width="14.44140625" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
-    <col min="10" max="11" width="10.36328125" customWidth="1"/>
-    <col min="12" max="12" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.7265625" customWidth="1"/>
+    <col min="10" max="11" width="10.33203125" customWidth="1"/>
+    <col min="12" max="12" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -636,7 +656,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -667,15 +687,15 @@
       <c r="J2" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K2" s="3" t="b">
-        <v>1</v>
+      <c r="K2" s="9" t="s">
+        <v>65</v>
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="str">
         <f>A2</f>
         <v>Red</v>
@@ -707,8 +727,8 @@
       <c r="J3" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="K3" s="3" t="b">
-        <v>0</v>
+      <c r="K3" s="9" t="s">
+        <v>66</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3" t="str">
@@ -716,7 +736,7 @@
         <v>1, 3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="str">
         <f t="shared" ref="A4:A67" si="0">A3</f>
         <v>Red</v>
@@ -757,7 +777,7 @@
         <v>2, 4</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -798,7 +818,7 @@
         <v>3, 5</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -839,7 +859,7 @@
         <v>4, 6</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -880,7 +900,7 @@
         <v>5, 7</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -923,7 +943,7 @@
         <v>6, 8</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -964,7 +984,7 @@
         <v>7, 9</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -1004,7 +1024,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -1044,7 +1064,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -1085,7 +1105,7 @@
         <v>10, 12</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -1126,7 +1146,7 @@
         <v>11, 13</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -1167,7 +1187,7 @@
         <v>12, 14</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -1208,7 +1228,7 @@
         <v>13, 15</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -1248,7 +1268,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -1290,7 +1310,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -1331,7 +1351,7 @@
         <v>16, 18</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -1373,7 +1393,7 @@
         <v>17, 19</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -1414,7 +1434,7 @@
         <v>18, 20</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -1455,7 +1475,7 @@
         <v>19, 21</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -1498,7 +1518,7 @@
         <v>20, 22</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -1539,7 +1559,7 @@
         <v>21, 23</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -1580,7 +1600,7 @@
         <v>22, 24</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -1621,7 +1641,7 @@
         <v>23, 25</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -1664,7 +1684,7 @@
         <v>24, 26</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -1705,7 +1725,7 @@
         <v>25, 27</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -1745,7 +1765,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -1785,7 +1805,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -1826,7 +1846,7 @@
         <v>28, 30</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -1867,7 +1887,7 @@
         <v>29, 31</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -1908,7 +1928,7 @@
         <v>30, 32</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -1948,7 +1968,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -1988,7 +2008,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -2029,7 +2049,7 @@
         <v>33, 35</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -2072,7 +2092,7 @@
         <v>34, 36</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -2113,7 +2133,7 @@
         <v>35, 37</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -2154,7 +2174,7 @@
         <v>36, 38</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -2194,7 +2214,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -2234,7 +2254,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -2275,7 +2295,7 @@
         <v>39, 41</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -2316,7 +2336,7 @@
         <v>40, 42</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -2357,7 +2377,7 @@
         <v>41, 43</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -2397,7 +2417,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -2437,7 +2457,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -2480,7 +2500,7 @@
         <v>44, 46</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -2521,7 +2541,7 @@
         <v>45, 47</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -2562,7 +2582,7 @@
         <v>46, 48</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -2605,7 +2625,7 @@
         <v>47, 49</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -2646,7 +2666,7 @@
         <v>48, 50</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -2687,7 +2707,7 @@
         <v>49, 51</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -2728,7 +2748,7 @@
         <v>50, 52</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -2768,7 +2788,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -2808,7 +2828,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -2849,7 +2869,7 @@
         <v>53, 55</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -2890,7 +2910,7 @@
         <v>54, 56</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -2931,7 +2951,7 @@
         <v>55, 57</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -2972,7 +2992,7 @@
         <v>56, 58</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -3013,7 +3033,7 @@
         <v>57, 59</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -3054,7 +3074,7 @@
         <v>58, 60</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -3097,7 +3117,7 @@
         <v>59, 61</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -3138,7 +3158,7 @@
         <v>60, 62</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -3179,7 +3199,7 @@
         <v>61, 63</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -3220,7 +3240,7 @@
         <v>62, 64</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -3261,7 +3281,7 @@
         <v>63, 65</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -3302,7 +3322,7 @@
         <v>64, 66</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
@@ -3342,7 +3362,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="str">
         <f t="shared" ref="A68:A79" si="6">A67</f>
         <v>Red</v>
@@ -3382,7 +3402,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="str">
         <f t="shared" si="6"/>
         <v>Red</v>
@@ -3423,7 +3443,7 @@
         <v>67, 69</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="str">
         <f t="shared" si="6"/>
         <v>Red</v>
@@ -3464,7 +3484,7 @@
         <v>68, 70</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="str">
         <f t="shared" si="6"/>
         <v>Red</v>
@@ -3505,7 +3525,7 @@
         <v>69, 71</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="str">
         <f t="shared" si="6"/>
         <v>Red</v>
@@ -3545,7 +3565,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="str">
         <f t="shared" si="6"/>
         <v>Red</v>
@@ -3585,7 +3605,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="str">
         <f t="shared" si="6"/>
         <v>Red</v>
@@ -3626,7 +3646,7 @@
         <v>72, 74</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="str">
         <f t="shared" si="6"/>
         <v>Red</v>
@@ -3667,7 +3687,7 @@
         <v>73, 75</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="str">
         <f t="shared" si="6"/>
         <v>Red</v>
@@ -3708,7 +3728,7 @@
         <v>74, 76</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="str">
         <f t="shared" si="6"/>
         <v>Red</v>
@@ -3748,7 +3768,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="str">
         <f t="shared" si="6"/>
         <v>Red</v>
@@ -3788,7 +3808,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="str">
         <f t="shared" si="6"/>
         <v>Red</v>
@@ -3826,229 +3846,229 @@
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C80" s="6"/>
     </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C81" s="6"/>
     </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C82" s="6"/>
     </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C83" s="6"/>
     </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C84" s="6"/>
     </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C85" s="6"/>
     </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C86" s="6"/>
     </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C87" s="6"/>
     </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C88" s="6"/>
     </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C89" s="6"/>
     </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C90" s="6"/>
     </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C91" s="6"/>
     </row>
-    <row r="92" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C92" s="6"/>
     </row>
-    <row r="93" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C93" s="6"/>
     </row>
-    <row r="94" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C94" s="6"/>
     </row>
-    <row r="95" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="95" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C95" s="6"/>
     </row>
-    <row r="96" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="96" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C96" s="6"/>
     </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C97" s="6"/>
     </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="98" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C98" s="6"/>
     </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="99" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C99" s="6"/>
     </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C100" s="6"/>
     </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="101" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C101" s="6"/>
     </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="102" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C102" s="6"/>
     </row>
-    <row r="103" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="103" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C103" s="6"/>
     </row>
-    <row r="104" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="104" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C104" s="6"/>
     </row>
-    <row r="105" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="105" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C105" s="6"/>
     </row>
-    <row r="106" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="106" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C106" s="6"/>
     </row>
-    <row r="107" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="107" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C107" s="6"/>
     </row>
-    <row r="108" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="108" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C108" s="6"/>
     </row>
-    <row r="109" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="109" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C109" s="6"/>
     </row>
-    <row r="110" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="110" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C110" s="6"/>
     </row>
-    <row r="111" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="111" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C111" s="6"/>
     </row>
-    <row r="112" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="112" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C112" s="6"/>
     </row>
-    <row r="113" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="113" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C113" s="6"/>
     </row>
-    <row r="114" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="114" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C114" s="6"/>
     </row>
-    <row r="115" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="115" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C115" s="6"/>
     </row>
-    <row r="116" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="116" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C116" s="6"/>
     </row>
-    <row r="117" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="117" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C117" s="6"/>
     </row>
-    <row r="118" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="118" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C118" s="6"/>
     </row>
-    <row r="119" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="119" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C119" s="6"/>
     </row>
-    <row r="120" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="120" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C120" s="6"/>
     </row>
-    <row r="121" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="121" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C121" s="6"/>
     </row>
-    <row r="122" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="122" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C122" s="6"/>
     </row>
-    <row r="123" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="123" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C123" s="6"/>
     </row>
-    <row r="124" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="124" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C124" s="6"/>
     </row>
-    <row r="125" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="125" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C125" s="6"/>
     </row>
-    <row r="126" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="126" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C126" s="6"/>
     </row>
-    <row r="127" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="127" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C127" s="6"/>
     </row>
-    <row r="128" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="128" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C128" s="6"/>
     </row>
-    <row r="129" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="129" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C129" s="6"/>
     </row>
-    <row r="130" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="130" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C130" s="6"/>
     </row>
-    <row r="131" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="131" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C131" s="6"/>
     </row>
-    <row r="132" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="132" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C132" s="6"/>
     </row>
-    <row r="133" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="133" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C133" s="6"/>
     </row>
-    <row r="134" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="134" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C134" s="6"/>
     </row>
-    <row r="135" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="135" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C135" s="6"/>
     </row>
-    <row r="136" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="136" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C136" s="6"/>
     </row>
-    <row r="137" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="137" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C137" s="6"/>
     </row>
-    <row r="138" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="138" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C138" s="6"/>
     </row>
-    <row r="139" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="139" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C139" s="6"/>
     </row>
-    <row r="140" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="140" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C140" s="6"/>
     </row>
-    <row r="141" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="141" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C141" s="6"/>
     </row>
-    <row r="142" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="142" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C142" s="6"/>
     </row>
-    <row r="143" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="143" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C143" s="6"/>
     </row>
-    <row r="144" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="144" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C144" s="6"/>
     </row>
-    <row r="145" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="145" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C145" s="6"/>
     </row>
-    <row r="146" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="146" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C146" s="6"/>
     </row>
-    <row r="147" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="147" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C147" s="6"/>
     </row>
-    <row r="148" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="148" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C148" s="6"/>
     </row>
-    <row r="149" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="149" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C149" s="6"/>
     </row>
-    <row r="150" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="150" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C150" s="6"/>
     </row>
-    <row r="151" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="151" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C151" s="6"/>
     </row>
-    <row r="152" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="152" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C152" s="6"/>
     </row>
-    <row r="153" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="153" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C153" s="6"/>
     </row>
-    <row r="154" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="154" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C154" s="6"/>
     </row>
   </sheetData>

</xml_diff>